<commit_message>
Add multiple stocks to the tracker. Saved the stocks in seperate sheets in the Excel file.
</commit_message>
<xml_diff>
--- a/tesla_stock_data.xlsx
+++ b/tesla_stock_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -767,6 +767,26 @@
         <v>296.97</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11:23:03</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>$298.26</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>298.26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>